<commit_message>
Got the logging services deployment working.  Added the deploy monitoring services scripts...they still need some love
</commit_message>
<xml_diff>
--- a/wiki/cost-estimates/emr-cost-estimator.xlsx
+++ b/wiki/cost-estimates/emr-cost-estimator.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>S3</t>
   </si>
@@ -69,9 +69,6 @@
     <t>m4.large</t>
   </si>
   <si>
-    <t>Price Per Hour</t>
-  </si>
-  <si>
     <t># of Instances</t>
   </si>
   <si>
@@ -106,6 +103,15 @@
   </si>
   <si>
     <t>Total Storage Price</t>
+  </si>
+  <si>
+    <t>Price Per Hour EC2</t>
+  </si>
+  <si>
+    <t>Price Per Hour EMR</t>
+  </si>
+  <si>
+    <t>Total Price Per Hour</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="B2:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="B2:D3"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2B148D-022F-4E13-B82B-09BB70200B43}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,15 +524,17 @@
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" customWidth="1"/>
-    <col min="14" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" customWidth="1"/>
+    <col min="16" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -534,12 +542,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -547,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>1500</v>
       </c>
@@ -561,12 +569,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -574,34 +582,40 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>25</v>
       </c>
-      <c r="L9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -612,35 +626,41 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f>B1</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10">
         <f>D10*E10*F10</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="I10" s="1">
-        <f>G10*H10</f>
-        <v>0.24</v>
-      </c>
-      <c r="J10">
+        <v>0.06</v>
+      </c>
+      <c r="J10" s="1">
+        <f>H10+I10</f>
+        <v>0.26</v>
+      </c>
+      <c r="K10" s="1">
+        <f>G10*J10</f>
+        <v>5.2</v>
+      </c>
+      <c r="L10">
         <v>20</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>0.1</v>
       </c>
-      <c r="L10">
-        <f>J10*K10*E10</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <f>L10*M10*E10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -648,73 +668,79 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E11">
-        <f>B1</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="G11">
         <f>D11*E11*F11</f>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="1">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="I11" s="1">
-        <f>G11*H11</f>
-        <v>24</v>
-      </c>
-      <c r="J11">
+        <v>0.06</v>
+      </c>
+      <c r="J11" s="1">
+        <f>H11+I11</f>
+        <v>0.26</v>
+      </c>
+      <c r="K11" s="1">
+        <f>G11*J11</f>
+        <v>260</v>
+      </c>
+      <c r="L11">
         <v>20</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>0.1</v>
       </c>
-      <c r="L11">
-        <f>J11*K11*E11</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I13" s="1">
-        <f>SUM(I10:I11)</f>
-        <v>24.24</v>
-      </c>
-      <c r="L13">
-        <f>SUM(L10:L11)</f>
-        <v>8</v>
-      </c>
-      <c r="N13" s="1">
-        <f>SUM(I13:L13)</f>
-        <v>32.239999999999995</v>
-      </c>
-      <c r="O13" s="1">
-        <f>N13+D6</f>
-        <v>47.239999999999995</v>
+      <c r="N11">
+        <f>L11*M11*E11</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <f>SUM(K10:K11)</f>
+        <v>265.2</v>
+      </c>
+      <c r="N13">
+        <f>SUM(N10:N11)</f>
+        <v>20</v>
+      </c>
+      <c r="P13" s="1">
+        <f>SUM(K13:N13)</f>
+        <v>285.2</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>P13+D6</f>
+        <v>300.2</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>